<commit_message>
xy large area scan bad
clone matrix before saving
</commit_message>
<xml_diff>
--- a/Project_AFM_Controller_USB/parameterPID.xlsx
+++ b/Project_AFM_Controller_USB/parameterPID.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>P</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>I 增大 加大惯性 造成超调</t>
+  </si>
+  <si>
+    <t>imporved for close loop</t>
   </si>
 </sst>
 </file>
@@ -90,6 +93,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -106,7 +177,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -385,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E9"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,6 +541,72 @@
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>0.4</v>
+      </c>
+      <c r="E14">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+      <c r="E15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.2000000000000001E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dynamic code, auto task
</commit_message>
<xml_diff>
--- a/Project_AFM_Controller_USB/parameterPID.xlsx
+++ b/Project_AFM_Controller_USB/parameterPID.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>P</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>distance=20um</t>
+  </si>
+  <si>
+    <t>scanRate</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>30um,15um</t>
+  </si>
+  <si>
+    <t>15um</t>
   </si>
 </sst>
 </file>
@@ -67,12 +79,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,9 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E23"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +583,7 @@
       <c r="C13">
         <v>0.2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13">
@@ -577,7 +597,7 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.4</v>
       </c>
       <c r="E14">
@@ -591,7 +611,7 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0.3</v>
       </c>
       <c r="E15">
@@ -605,65 +625,117 @@
       <c r="C16" s="1">
         <v>1E-4</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="E16" s="1">
         <v>2.2000000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20160902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>0.2</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S28" t="s">
         <v>4</v>
       </c>
-      <c r="C20">
+      <c r="T28">
         <v>0.3</v>
       </c>
-      <c r="D20">
+      <c r="U28">
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S29" t="s">
         <v>0</v>
       </c>
-      <c r="C21">
+      <c r="T29">
         <v>0.1</v>
       </c>
-      <c r="D21">
+      <c r="U29">
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S30" t="s">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="T30">
         <v>0.09</v>
       </c>
-      <c r="D22">
+      <c r="U30">
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S31" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="1">
+      <c r="T31" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D23" s="1">
+      <c r="U31" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>